<commit_message>
changes in meta-data (compliance with guidelines)
</commit_message>
<xml_diff>
--- a/Metadata_Craving_20220913.xlsx
+++ b/Metadata_Craving_20220913.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leonie.koban/Dropbox/work/BOULDER_PROJECTS/15_Craving/A_Data_Code_FINAL_cleaned/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leonie.koban/Dropbox/work/tools/GitHub/NCS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83641ED-AF98-D44A-A6B8-C0B52177C702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328A0093-DDA6-3648-A2DE-3B5AB650F07F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16740" xr2:uid="{15491F0C-9429-F543-892A-7566671FE80D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="36">
   <si>
     <t>Folds (cv)</t>
   </si>
@@ -144,9 +144,6 @@
   </si>
   <si>
     <t>Predicted rating (out-of-sample NCS response)</t>
-  </si>
-  <si>
-    <t>NaN</t>
   </si>
 </sst>
 </file>
@@ -1172,7 +1169,7 @@
   <dimension ref="A1:AA169"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J101" sqref="J3:J101"/>
+      <selection activeCell="H3" sqref="H3:J101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1309,15 +1306,9 @@
       <c r="G3" s="18">
         <v>0</v>
       </c>
-      <c r="H3" s="18">
-        <v>38</v>
-      </c>
-      <c r="I3" s="20">
-        <v>33.961352657004831</v>
-      </c>
-      <c r="J3" s="18">
-        <v>12</v>
-      </c>
+      <c r="H3" s="18"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="18"/>
       <c r="K3" s="21">
         <v>8.9870559907454101E-2</v>
       </c>
@@ -1379,15 +1370,9 @@
       <c r="G4" s="18">
         <v>1</v>
       </c>
-      <c r="H4" s="18">
-        <v>28</v>
-      </c>
-      <c r="I4" s="20">
-        <v>25.544843520268849</v>
-      </c>
-      <c r="J4" s="18">
-        <v>13</v>
-      </c>
+      <c r="H4" s="18"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="18"/>
       <c r="K4" s="21">
         <v>8.8285795816877094E-2</v>
       </c>
@@ -1449,15 +1434,9 @@
       <c r="G5" s="18">
         <v>0</v>
       </c>
-      <c r="H5" s="18">
-        <v>23</v>
-      </c>
-      <c r="I5" s="20">
-        <v>21.871111111111109</v>
-      </c>
-      <c r="J5" s="18">
-        <v>15</v>
-      </c>
+      <c r="H5" s="18"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="18"/>
       <c r="K5" s="21">
         <v>8.4537293645661399E-2</v>
       </c>
@@ -1519,15 +1498,9 @@
       <c r="G6" s="18">
         <v>1</v>
       </c>
-      <c r="H6" s="18">
-        <v>23</v>
-      </c>
-      <c r="I6" s="20">
-        <v>28.126081314878896</v>
-      </c>
-      <c r="J6" s="18">
-        <v>15</v>
-      </c>
+      <c r="H6" s="18"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="18"/>
       <c r="K6" s="21">
         <v>0.11304542243275501</v>
       </c>
@@ -1589,15 +1562,9 @@
       <c r="G7" s="18">
         <v>1</v>
       </c>
-      <c r="H7" s="18">
-        <v>29</v>
-      </c>
-      <c r="I7" s="20">
-        <v>21.697530864197528</v>
-      </c>
-      <c r="J7" s="18">
-        <v>14</v>
-      </c>
+      <c r="H7" s="18"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="18"/>
       <c r="K7" s="21">
         <v>6.4399700163505894E-2</v>
       </c>
@@ -1659,15 +1626,9 @@
       <c r="G8" s="18">
         <v>0</v>
       </c>
-      <c r="H8" s="18">
-        <v>28</v>
-      </c>
-      <c r="I8" s="20">
-        <v>32.817515432098766</v>
-      </c>
-      <c r="J8" s="18">
-        <v>14</v>
-      </c>
+      <c r="H8" s="18"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="18"/>
       <c r="K8" s="21">
         <v>5.8401311601280703E-2</v>
       </c>
@@ -1729,15 +1690,9 @@
       <c r="G9" s="18">
         <v>1</v>
       </c>
-      <c r="H9" s="18">
-        <v>43</v>
-      </c>
-      <c r="I9" s="20">
-        <v>26.831081081081081</v>
-      </c>
-      <c r="J9" s="18">
-        <v>14</v>
-      </c>
+      <c r="H9" s="18"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="18"/>
       <c r="K9" s="21">
         <v>4.4336456507138799E-2</v>
       </c>
@@ -1799,15 +1754,9 @@
       <c r="G10" s="18">
         <v>0</v>
       </c>
-      <c r="H10" s="18">
-        <v>50</v>
-      </c>
-      <c r="I10" s="20">
-        <v>28.286390532544377</v>
-      </c>
-      <c r="J10" s="18">
-        <v>16</v>
-      </c>
+      <c r="H10" s="18"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="18"/>
       <c r="K10" s="21">
         <v>0.12001437431109099</v>
       </c>
@@ -1869,15 +1818,9 @@
       <c r="G11" s="18">
         <v>1</v>
       </c>
-      <c r="H11" s="18">
-        <v>55</v>
-      </c>
-      <c r="I11" s="20">
-        <v>26.254897959183673</v>
-      </c>
-      <c r="J11" s="18">
-        <v>16</v>
-      </c>
+      <c r="H11" s="18"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="18"/>
       <c r="K11" s="21">
         <v>0.110416106778228</v>
       </c>
@@ -1939,15 +1882,9 @@
       <c r="G12" s="18">
         <v>0</v>
       </c>
-      <c r="H12" s="18">
-        <v>24</v>
-      </c>
-      <c r="I12" s="20">
-        <v>22.707730006683004</v>
-      </c>
-      <c r="J12" s="18">
-        <v>15</v>
-      </c>
+      <c r="H12" s="18"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="18"/>
       <c r="K12" s="21">
         <v>8.9909306045520498E-2</v>
       </c>
@@ -2009,15 +1946,9 @@
       <c r="G13" s="18">
         <v>0</v>
       </c>
-      <c r="H13" s="18">
-        <v>26</v>
-      </c>
-      <c r="I13" s="20">
-        <v>32.446153846153848</v>
-      </c>
-      <c r="J13" s="18">
-        <v>14</v>
-      </c>
+      <c r="H13" s="18"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="18"/>
       <c r="K13" s="21">
         <v>0.106373584239931</v>
       </c>
@@ -2079,15 +2010,9 @@
       <c r="G14" s="18">
         <v>1</v>
       </c>
-      <c r="H14" s="18">
-        <v>50</v>
-      </c>
-      <c r="I14" s="20">
-        <v>26.578449905482042</v>
-      </c>
-      <c r="J14" s="18">
-        <v>12</v>
-      </c>
+      <c r="H14" s="18"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="18"/>
       <c r="K14" s="21">
         <v>0.14394745824114</v>
       </c>
@@ -2149,15 +2074,9 @@
       <c r="G15" s="18">
         <v>0</v>
       </c>
-      <c r="H15" s="18">
-        <v>32</v>
-      </c>
-      <c r="I15" s="20">
-        <v>24.12662721893491</v>
-      </c>
-      <c r="J15" s="18">
-        <v>16</v>
-      </c>
+      <c r="H15" s="18"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="18"/>
       <c r="K15" s="21">
         <v>6.3087822983423303E-2</v>
       </c>
@@ -2219,15 +2138,9 @@
       <c r="G16" s="18">
         <v>1</v>
       </c>
-      <c r="H16" s="18">
-        <v>22</v>
-      </c>
-      <c r="I16" s="20">
-        <v>28.793320730938877</v>
-      </c>
-      <c r="J16" s="18">
-        <v>14</v>
-      </c>
+      <c r="H16" s="18"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="18"/>
       <c r="K16" s="21">
         <v>6.8977783038315699E-2</v>
       </c>
@@ -2289,15 +2202,9 @@
       <c r="G17" s="18">
         <v>1</v>
       </c>
-      <c r="H17" s="18">
-        <v>44</v>
-      </c>
-      <c r="I17" s="20">
-        <v>28.47800925925926</v>
-      </c>
-      <c r="J17" s="18">
-        <v>15</v>
-      </c>
+      <c r="H17" s="18"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="18"/>
       <c r="K17" s="21">
         <v>0.12013046942436</v>
       </c>
@@ -2359,15 +2266,9 @@
       <c r="G18" s="18">
         <v>1</v>
       </c>
-      <c r="H18" s="18">
-        <v>25</v>
-      </c>
-      <c r="I18" s="20">
-        <v>19.244991073199763</v>
-      </c>
-      <c r="J18" s="18">
-        <v>14</v>
-      </c>
+      <c r="H18" s="18"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="18"/>
       <c r="K18" s="21">
         <v>4.8227244590077697E-2</v>
       </c>
@@ -2429,15 +2330,9 @@
       <c r="G19" s="18">
         <v>1</v>
       </c>
-      <c r="H19" s="18">
-        <v>27</v>
-      </c>
-      <c r="I19" s="20">
-        <v>31.008191556395715</v>
-      </c>
-      <c r="J19" s="18">
-        <v>14</v>
-      </c>
+      <c r="H19" s="18"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="18"/>
       <c r="K19" s="21">
         <v>0.10169557001167299</v>
       </c>
@@ -2499,15 +2394,9 @@
       <c r="G20" s="18">
         <v>1</v>
       </c>
-      <c r="H20" s="18">
-        <v>45</v>
-      </c>
-      <c r="I20" s="20">
-        <v>25.675101099999999</v>
-      </c>
-      <c r="J20" s="18">
-        <v>12</v>
-      </c>
+      <c r="H20" s="18"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="18"/>
       <c r="K20" s="21">
         <v>4.3173407625563001E-2</v>
       </c>
@@ -2569,15 +2458,9 @@
       <c r="G21" s="18">
         <v>1</v>
       </c>
-      <c r="H21" s="18">
-        <v>48</v>
-      </c>
-      <c r="I21" s="20">
-        <v>22.262876899999998</v>
-      </c>
-      <c r="J21" s="18">
-        <v>12</v>
-      </c>
+      <c r="H21" s="18"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="18"/>
       <c r="K21" s="21">
         <v>9.4766390753220103E-2</v>
       </c>
@@ -2639,15 +2522,9 @@
       <c r="G22" s="18">
         <v>1</v>
       </c>
-      <c r="H22" s="18">
-        <v>36</v>
-      </c>
-      <c r="I22" s="20">
-        <v>34.602074199999997</v>
-      </c>
-      <c r="J22" s="18">
-        <v>11</v>
-      </c>
+      <c r="H22" s="18"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="18"/>
       <c r="K22" s="21">
         <v>6.6446392048269201E-2</v>
       </c>
@@ -2709,15 +2586,9 @@
       <c r="G23" s="18">
         <v>1</v>
       </c>
-      <c r="H23" s="18">
-        <v>43</v>
-      </c>
-      <c r="I23" s="20">
-        <v>23.148149400000001</v>
-      </c>
-      <c r="J23" s="18">
-        <v>13</v>
-      </c>
+      <c r="H23" s="18"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="18"/>
       <c r="K23" s="21">
         <v>0.13538456098995499</v>
       </c>
@@ -2779,15 +2650,9 @@
       <c r="G24" s="18">
         <v>1</v>
       </c>
-      <c r="H24" s="18">
-        <v>45</v>
-      </c>
-      <c r="I24" s="20">
-        <v>30.722224099999998</v>
-      </c>
-      <c r="J24" s="18">
-        <v>12</v>
-      </c>
+      <c r="H24" s="18"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="18"/>
       <c r="K24" s="21">
         <v>0.36114434412489699</v>
       </c>
@@ -2849,15 +2714,9 @@
       <c r="G25" s="18">
         <v>1</v>
       </c>
-      <c r="H25" s="18">
-        <v>45</v>
-      </c>
-      <c r="I25" s="20">
-        <v>39.318335900000001</v>
-      </c>
-      <c r="J25" s="18">
-        <v>12</v>
-      </c>
+      <c r="H25" s="18"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="18"/>
       <c r="K25" s="21">
         <v>9.0660562940965098E-2</v>
       </c>
@@ -2919,15 +2778,9 @@
       <c r="G26" s="18">
         <v>1</v>
       </c>
-      <c r="H26" s="18">
-        <v>42</v>
-      </c>
-      <c r="I26" s="20">
-        <v>33.179014100000003</v>
-      </c>
-      <c r="J26" s="18">
-        <v>12</v>
-      </c>
+      <c r="H26" s="18"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="18"/>
       <c r="K26" s="21">
         <v>8.5118623109490602E-2</v>
       </c>
@@ -2989,15 +2842,9 @@
       <c r="G27" s="18">
         <v>1</v>
       </c>
-      <c r="H27" s="18">
-        <v>41</v>
-      </c>
-      <c r="I27" s="20">
-        <v>30.092594200000001</v>
-      </c>
-      <c r="J27" s="18">
-        <v>11</v>
-      </c>
+      <c r="H27" s="18"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="18"/>
       <c r="K27" s="21">
         <v>6.8623117578546194E-2</v>
       </c>
@@ -3059,15 +2906,9 @@
       <c r="G28" s="18">
         <v>1</v>
       </c>
-      <c r="H28" s="18">
-        <v>48</v>
-      </c>
-      <c r="I28" s="20">
-        <v>24.557981699999999</v>
-      </c>
-      <c r="J28" s="18">
-        <v>11</v>
-      </c>
+      <c r="H28" s="18"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="18"/>
       <c r="K28" s="21">
         <v>9.6818032106822896E-2</v>
       </c>
@@ -3129,15 +2970,9 @@
       <c r="G29" s="18">
         <v>1</v>
       </c>
-      <c r="H29" s="18">
-        <v>46</v>
-      </c>
-      <c r="I29" s="20">
-        <v>22.80864365</v>
-      </c>
-      <c r="J29" s="18">
-        <v>12</v>
-      </c>
+      <c r="H29" s="18"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="18"/>
       <c r="K29" s="21">
         <v>5.31449913948666E-2</v>
       </c>
@@ -3199,15 +3034,9 @@
       <c r="G30" s="18">
         <v>1</v>
       </c>
-      <c r="H30" s="18">
-        <v>48</v>
-      </c>
-      <c r="I30" s="20">
-        <v>29.92362095</v>
-      </c>
-      <c r="J30" s="18">
-        <v>12</v>
-      </c>
+      <c r="H30" s="18"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="18"/>
       <c r="K30" s="21">
         <v>0.12823190693895301</v>
       </c>
@@ -3269,15 +3098,9 @@
       <c r="G31" s="18">
         <v>0</v>
       </c>
-      <c r="H31" s="18">
-        <v>30</v>
-      </c>
-      <c r="I31" s="20">
-        <v>23.372576760000001</v>
-      </c>
-      <c r="J31" s="18">
-        <v>12</v>
-      </c>
+      <c r="H31" s="18"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="18"/>
       <c r="K31" s="21">
         <v>6.3321440843706001E-2</v>
       </c>
@@ -3339,15 +3162,9 @@
       <c r="G32" s="18">
         <v>1</v>
       </c>
-      <c r="H32" s="18">
-        <v>49</v>
-      </c>
-      <c r="I32" s="20">
-        <v>35.785464490000003</v>
-      </c>
-      <c r="J32" s="18">
-        <v>12</v>
-      </c>
+      <c r="H32" s="18"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="18"/>
       <c r="K32" s="21">
         <v>0.112092078777381</v>
       </c>
@@ -3409,15 +3226,9 @@
       <c r="G33" s="18">
         <v>1</v>
       </c>
-      <c r="H33" s="18">
-        <v>49</v>
-      </c>
-      <c r="I33" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="J33" s="18">
-        <v>15</v>
-      </c>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
       <c r="K33" s="21">
         <v>6.0802895440580498E-2</v>
       </c>
@@ -3479,15 +3290,9 @@
       <c r="G34" s="18">
         <v>0</v>
       </c>
-      <c r="H34" s="18">
-        <v>29</v>
-      </c>
-      <c r="I34" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="J34" s="18">
-        <v>12</v>
-      </c>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
       <c r="K34" s="21">
         <v>3.5432939606493602E-2</v>
       </c>
@@ -3549,15 +3354,9 @@
       <c r="G35" s="18">
         <v>1</v>
       </c>
-      <c r="H35" s="18">
-        <v>36</v>
-      </c>
-      <c r="I35" s="20">
-        <v>26.69477109</v>
-      </c>
-      <c r="J35" s="18">
-        <v>14</v>
-      </c>
+      <c r="H35" s="18"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="18"/>
       <c r="K35" s="21">
         <v>4.3856278537296803E-2</v>
       </c>
@@ -3619,15 +3418,9 @@
       <c r="G36" s="18">
         <v>0</v>
       </c>
-      <c r="H36" s="18">
-        <v>49</v>
-      </c>
-      <c r="I36" s="20">
-        <v>43.356166440000003</v>
-      </c>
-      <c r="J36" s="18">
-        <v>16</v>
-      </c>
+      <c r="H36" s="18"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="18"/>
       <c r="K36" s="21">
         <v>0.127246979512259</v>
       </c>
@@ -3689,15 +3482,9 @@
       <c r="G37" s="18">
         <v>1</v>
       </c>
-      <c r="H37" s="18">
-        <v>46</v>
-      </c>
-      <c r="I37" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="J37" s="18">
-        <v>15</v>
-      </c>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="18"/>
       <c r="K37" s="21">
         <v>0.114820201882446</v>
       </c>
@@ -3759,15 +3546,9 @@
       <c r="G38" s="18">
         <v>1</v>
       </c>
-      <c r="H38" s="18">
-        <v>44</v>
-      </c>
-      <c r="I38" s="20">
-        <v>29.48096615</v>
-      </c>
-      <c r="J38" s="18">
-        <v>16</v>
-      </c>
+      <c r="H38" s="18"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="18"/>
       <c r="K38" s="21">
         <v>0.35940177284505997</v>
       </c>
@@ -3829,15 +3610,9 @@
       <c r="G39" s="18">
         <v>1</v>
       </c>
-      <c r="H39" s="18">
-        <v>46</v>
-      </c>
-      <c r="I39" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="J39" s="18">
-        <v>11</v>
-      </c>
+      <c r="H39" s="18"/>
+      <c r="I39" s="18"/>
+      <c r="J39" s="18"/>
       <c r="K39" s="21">
         <v>0.16384438560001099</v>
       </c>
@@ -3899,15 +3674,9 @@
       <c r="G40" s="18">
         <v>1</v>
       </c>
-      <c r="H40" s="18">
-        <v>49</v>
-      </c>
-      <c r="I40" s="20">
-        <v>30.260241879999999</v>
-      </c>
-      <c r="J40" s="18">
-        <v>11</v>
-      </c>
+      <c r="H40" s="18"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="18"/>
       <c r="K40" s="21">
         <v>9.5620226590209301E-2</v>
       </c>
@@ -3969,15 +3738,9 @@
       <c r="G41" s="18">
         <v>0</v>
       </c>
-      <c r="H41" s="18">
-        <v>44</v>
-      </c>
-      <c r="I41" s="20">
-        <v>31.618202499999999</v>
-      </c>
-      <c r="J41" s="18">
-        <v>16</v>
-      </c>
+      <c r="H41" s="18"/>
+      <c r="I41" s="20"/>
+      <c r="J41" s="18"/>
       <c r="K41" s="21">
         <v>0.202066346524131</v>
       </c>
@@ -4039,15 +3802,9 @@
       <c r="G42" s="18">
         <v>1</v>
       </c>
-      <c r="H42" s="18">
-        <v>47</v>
-      </c>
-      <c r="I42" s="20">
-        <v>24.5740923</v>
-      </c>
-      <c r="J42" s="18">
-        <v>19</v>
-      </c>
+      <c r="H42" s="18"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="18"/>
       <c r="K42" s="21">
         <v>6.1940894439751003E-2</v>
       </c>
@@ -4109,15 +3866,9 @@
       <c r="G43" s="18">
         <v>1</v>
       </c>
-      <c r="H43" s="18">
-        <v>47</v>
-      </c>
-      <c r="I43" s="20">
-        <v>27.051901699999998</v>
-      </c>
-      <c r="J43" s="18">
-        <v>14</v>
-      </c>
+      <c r="H43" s="18"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="18"/>
       <c r="K43" s="21">
         <v>0.30323516179931798</v>
       </c>
@@ -4179,15 +3930,9 @@
       <c r="G44" s="18">
         <v>1</v>
       </c>
-      <c r="H44" s="18">
-        <v>42</v>
-      </c>
-      <c r="I44" s="20">
-        <v>22.761995599999999</v>
-      </c>
-      <c r="J44" s="18">
-        <v>13</v>
-      </c>
+      <c r="H44" s="18"/>
+      <c r="I44" s="20"/>
+      <c r="J44" s="18"/>
       <c r="K44" s="21">
         <v>6.5512269868825301E-2</v>
       </c>
@@ -4249,15 +3994,9 @@
       <c r="G45" s="18">
         <v>0</v>
       </c>
-      <c r="H45" s="18">
-        <v>38</v>
-      </c>
-      <c r="I45" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="J45" s="18">
-        <v>14</v>
-      </c>
+      <c r="H45" s="18"/>
+      <c r="I45" s="18"/>
+      <c r="J45" s="18"/>
       <c r="K45" s="21">
         <v>5.4969957878561002E-2</v>
       </c>
@@ -4319,15 +4058,9 @@
       <c r="G46" s="18">
         <v>1</v>
       </c>
-      <c r="H46" s="18">
-        <v>37</v>
-      </c>
-      <c r="I46" s="20">
-        <v>33.921584099999997</v>
-      </c>
-      <c r="J46" s="18">
-        <v>14</v>
-      </c>
+      <c r="H46" s="18"/>
+      <c r="I46" s="20"/>
+      <c r="J46" s="18"/>
       <c r="K46" s="21">
         <v>8.8840281701616203E-2</v>
       </c>
@@ -4389,15 +4122,9 @@
       <c r="G47" s="18">
         <v>1</v>
       </c>
-      <c r="H47" s="18">
-        <v>47</v>
-      </c>
-      <c r="I47" s="20">
-        <v>29.840191990000001</v>
-      </c>
-      <c r="J47" s="18">
-        <v>16</v>
-      </c>
+      <c r="H47" s="18"/>
+      <c r="I47" s="20"/>
+      <c r="J47" s="18"/>
       <c r="K47" s="21">
         <v>0.163111843037611</v>
       </c>
@@ -4459,15 +4186,9 @@
       <c r="G48" s="18">
         <v>0</v>
       </c>
-      <c r="H48" s="18">
-        <v>41</v>
-      </c>
-      <c r="I48" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="J48" s="18">
-        <v>17</v>
-      </c>
+      <c r="H48" s="18"/>
+      <c r="I48" s="18"/>
+      <c r="J48" s="18"/>
       <c r="K48" s="21">
         <v>4.1520749281218898E-2</v>
       </c>
@@ -4529,15 +4250,9 @@
       <c r="G49" s="18">
         <v>0</v>
       </c>
-      <c r="H49" s="18">
-        <v>48</v>
-      </c>
-      <c r="I49" s="20">
-        <v>20.02343625</v>
-      </c>
-      <c r="J49" s="18">
-        <v>17</v>
-      </c>
+      <c r="H49" s="18"/>
+      <c r="I49" s="20"/>
+      <c r="J49" s="18"/>
       <c r="K49" s="21">
         <v>3.9711461022668502E-2</v>
       </c>
@@ -4599,15 +4314,9 @@
       <c r="G50" s="18">
         <v>1</v>
       </c>
-      <c r="H50" s="18">
-        <v>49</v>
-      </c>
-      <c r="I50" s="20">
-        <v>30.85714286</v>
-      </c>
-      <c r="J50" s="18">
-        <v>14</v>
-      </c>
+      <c r="H50" s="18"/>
+      <c r="I50" s="20"/>
+      <c r="J50" s="18"/>
       <c r="K50" s="21">
         <v>0.15333512695780899</v>
       </c>
@@ -4669,15 +4378,9 @@
       <c r="G51" s="18">
         <v>0</v>
       </c>
-      <c r="H51" s="18">
-        <v>25</v>
-      </c>
-      <c r="I51" s="20">
-        <v>41.636716079999999</v>
-      </c>
-      <c r="J51" s="18">
-        <v>16</v>
-      </c>
+      <c r="H51" s="18"/>
+      <c r="I51" s="20"/>
+      <c r="J51" s="18"/>
       <c r="K51" s="21">
         <v>0.14722514359380701</v>
       </c>
@@ -4739,15 +4442,9 @@
       <c r="G52" s="18">
         <v>1</v>
       </c>
-      <c r="H52" s="18">
-        <v>39</v>
-      </c>
-      <c r="I52" s="20">
-        <v>24.475310879999999</v>
-      </c>
-      <c r="J52" s="18">
-        <v>18</v>
-      </c>
+      <c r="H52" s="18"/>
+      <c r="I52" s="20"/>
+      <c r="J52" s="18"/>
       <c r="K52" s="21">
         <v>4.7799170254909699E-2</v>
       </c>
@@ -4809,15 +4506,9 @@
       <c r="G53" s="18">
         <v>1</v>
       </c>
-      <c r="H53" s="18">
-        <v>44</v>
-      </c>
-      <c r="I53" s="20">
-        <v>23.696326429999999</v>
-      </c>
-      <c r="J53" s="18">
-        <v>14</v>
-      </c>
+      <c r="H53" s="18"/>
+      <c r="I53" s="20"/>
+      <c r="J53" s="18"/>
       <c r="K53" s="21">
         <v>0.100477126355077</v>
       </c>
@@ -4879,15 +4570,9 @@
       <c r="G54" s="18">
         <v>1</v>
       </c>
-      <c r="H54" s="18">
-        <v>44</v>
-      </c>
-      <c r="I54" s="20">
-        <v>32.478397819999998</v>
-      </c>
-      <c r="J54" s="18">
-        <v>14</v>
-      </c>
+      <c r="H54" s="18"/>
+      <c r="I54" s="20"/>
+      <c r="J54" s="18"/>
       <c r="K54" s="21">
         <v>0.41947408883722298</v>
       </c>
@@ -4949,15 +4634,9 @@
       <c r="G55" s="18">
         <v>1</v>
       </c>
-      <c r="H55" s="18">
-        <v>46</v>
-      </c>
-      <c r="I55" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="J55" s="18">
-        <v>14</v>
-      </c>
+      <c r="H55" s="18"/>
+      <c r="I55" s="18"/>
+      <c r="J55" s="18"/>
       <c r="K55" s="21">
         <v>0.117724221772724</v>
       </c>
@@ -5019,15 +4698,9 @@
       <c r="G56" s="18">
         <v>0</v>
       </c>
-      <c r="H56" s="18">
-        <v>39</v>
-      </c>
-      <c r="I56" s="20">
-        <v>43.530385819999999</v>
-      </c>
-      <c r="J56" s="18">
-        <v>12</v>
-      </c>
+      <c r="H56" s="18"/>
+      <c r="I56" s="20"/>
+      <c r="J56" s="18"/>
       <c r="K56" s="21">
         <v>0.107222802378887</v>
       </c>
@@ -5089,15 +4762,9 @@
       <c r="G57" s="18">
         <v>1</v>
       </c>
-      <c r="H57" s="18">
-        <v>42</v>
-      </c>
-      <c r="I57" s="20">
-        <v>29.3877551</v>
-      </c>
-      <c r="J57" s="18">
-        <v>16</v>
-      </c>
+      <c r="H57" s="18"/>
+      <c r="I57" s="20"/>
+      <c r="J57" s="18"/>
       <c r="K57" s="21">
         <v>7.2271795553638496E-2</v>
       </c>
@@ -5159,15 +4826,9 @@
       <c r="G58" s="18">
         <v>1</v>
       </c>
-      <c r="H58" s="18">
-        <v>38</v>
-      </c>
-      <c r="I58" s="20">
-        <v>27.689796909999998</v>
-      </c>
-      <c r="J58" s="18">
-        <v>18</v>
-      </c>
+      <c r="H58" s="18"/>
+      <c r="I58" s="20"/>
+      <c r="J58" s="18"/>
       <c r="K58" s="21">
         <v>8.4795232145134805E-2</v>
       </c>
@@ -5229,15 +4890,9 @@
       <c r="G59" s="18">
         <v>1</v>
       </c>
-      <c r="H59" s="17">
-        <v>44</v>
-      </c>
-      <c r="I59" s="20">
-        <v>21.80734693877551</v>
-      </c>
-      <c r="J59" s="18">
-        <v>17</v>
-      </c>
+      <c r="H59" s="17"/>
+      <c r="I59" s="20"/>
+      <c r="J59" s="18"/>
       <c r="K59" s="21">
         <v>5.0081687200878203E-2</v>
       </c>
@@ -5299,15 +4954,9 @@
       <c r="G60" s="18">
         <v>0</v>
       </c>
-      <c r="H60" s="17">
-        <v>43</v>
-      </c>
-      <c r="I60" s="20">
-        <v>24.45940828402367</v>
-      </c>
-      <c r="J60" s="18">
-        <v>16</v>
-      </c>
+      <c r="H60" s="17"/>
+      <c r="I60" s="20"/>
+      <c r="J60" s="18"/>
       <c r="K60" s="21">
         <v>7.0423764179544796E-2</v>
       </c>
@@ -5369,15 +5018,9 @@
       <c r="G61" s="18">
         <v>0</v>
       </c>
-      <c r="H61" s="17">
-        <v>26</v>
-      </c>
-      <c r="I61" s="22">
-        <v>26.948333333333331</v>
-      </c>
-      <c r="J61" s="18">
-        <v>17</v>
-      </c>
+      <c r="H61" s="17"/>
+      <c r="I61" s="22"/>
+      <c r="J61" s="18"/>
       <c r="K61" s="21">
         <v>4.4610010141446298E-2</v>
       </c>
@@ -5439,15 +5082,9 @@
       <c r="G62" s="18">
         <v>1</v>
       </c>
-      <c r="H62" s="17">
-        <v>45</v>
-      </c>
-      <c r="I62" s="20">
-        <v>20.466035502958579</v>
-      </c>
-      <c r="J62" s="18">
-        <v>16</v>
-      </c>
+      <c r="H62" s="17"/>
+      <c r="I62" s="20"/>
+      <c r="J62" s="18"/>
       <c r="K62" s="21">
         <v>0.20028028056542599</v>
       </c>
@@ -5509,15 +5146,9 @@
       <c r="G63" s="18">
         <v>1</v>
       </c>
-      <c r="H63" s="17">
-        <v>38</v>
-      </c>
-      <c r="I63" s="20">
-        <v>23.493243243243242</v>
-      </c>
-      <c r="J63" s="18">
-        <v>14</v>
-      </c>
+      <c r="H63" s="17"/>
+      <c r="I63" s="20"/>
+      <c r="J63" s="18"/>
       <c r="K63" s="21">
         <v>5.1956018293755298E-2</v>
       </c>
@@ -5579,15 +5210,9 @@
       <c r="G64" s="18">
         <v>1</v>
       </c>
-      <c r="H64" s="17">
-        <v>37</v>
-      </c>
-      <c r="I64" s="20">
-        <v>24.273780351971485</v>
-      </c>
-      <c r="J64" s="18">
-        <v>14</v>
-      </c>
+      <c r="H64" s="17"/>
+      <c r="I64" s="20"/>
+      <c r="J64" s="18"/>
       <c r="K64" s="21">
         <v>0.17200597953395699</v>
       </c>
@@ -5650,15 +5275,9 @@
       <c r="G65" s="18">
         <v>0</v>
       </c>
-      <c r="H65" s="17">
-        <v>20</v>
-      </c>
-      <c r="I65" s="20">
-        <v>19.737548828125</v>
-      </c>
-      <c r="J65" s="18">
-        <v>17</v>
-      </c>
+      <c r="H65" s="17"/>
+      <c r="I65" s="20"/>
+      <c r="J65" s="18"/>
       <c r="K65" s="21">
         <v>6.2279640835532397E-2</v>
       </c>
@@ -5721,15 +5340,9 @@
       <c r="G66" s="18">
         <v>0</v>
       </c>
-      <c r="H66" s="17">
-        <v>20</v>
-      </c>
-      <c r="I66" s="20">
-        <v>21.520408163265305</v>
-      </c>
-      <c r="J66" s="18">
-        <v>17</v>
-      </c>
+      <c r="H66" s="17"/>
+      <c r="I66" s="20"/>
+      <c r="J66" s="18"/>
       <c r="K66" s="21">
         <v>0.14587138305337199</v>
       </c>
@@ -5791,15 +5404,9 @@
       <c r="G67" s="18">
         <v>1</v>
       </c>
-      <c r="H67" s="17">
-        <v>25</v>
-      </c>
-      <c r="I67" s="20">
-        <v>23.490755179327241</v>
-      </c>
-      <c r="J67" s="18">
-        <v>16</v>
-      </c>
+      <c r="H67" s="17"/>
+      <c r="I67" s="20"/>
+      <c r="J67" s="18"/>
       <c r="K67" s="21">
         <v>3.9114514010341397E-2</v>
       </c>
@@ -5861,15 +5468,9 @@
       <c r="G68" s="18">
         <v>1</v>
       </c>
-      <c r="H68" s="17">
-        <v>24</v>
-      </c>
-      <c r="I68" s="20">
-        <v>21.107149559016701</v>
-      </c>
-      <c r="J68" s="18">
-        <v>15</v>
-      </c>
+      <c r="H68" s="17"/>
+      <c r="I68" s="20"/>
+      <c r="J68" s="18"/>
       <c r="K68" s="21">
         <v>2.1649221409170801E-2</v>
       </c>
@@ -5931,15 +5532,9 @@
       <c r="G69" s="18">
         <v>0</v>
       </c>
-      <c r="H69" s="17">
-        <v>23</v>
-      </c>
-      <c r="I69" s="20">
-        <v>23.490755179327241</v>
-      </c>
-      <c r="J69" s="18">
-        <v>17</v>
-      </c>
+      <c r="H69" s="17"/>
+      <c r="I69" s="20"/>
+      <c r="J69" s="18"/>
       <c r="K69" s="21">
         <v>7.3535222027404604E-2</v>
       </c>
@@ -6001,15 +5596,9 @@
       <c r="G70" s="18">
         <v>0</v>
       </c>
-      <c r="H70" s="17">
-        <v>18</v>
-      </c>
-      <c r="I70" s="20">
-        <v>21.96875</v>
-      </c>
-      <c r="J70" s="18">
-        <v>16</v>
-      </c>
+      <c r="H70" s="17"/>
+      <c r="I70" s="20"/>
+      <c r="J70" s="18"/>
       <c r="K70" s="21">
         <v>2.0772596377586199E-2</v>
       </c>
@@ -6071,15 +5660,9 @@
       <c r="G71" s="18">
         <v>1</v>
       </c>
-      <c r="H71" s="17">
-        <v>25</v>
-      </c>
-      <c r="I71" s="20">
-        <v>25.559210526315788</v>
-      </c>
-      <c r="J71" s="18">
-        <v>16</v>
-      </c>
+      <c r="H71" s="17"/>
+      <c r="I71" s="20"/>
+      <c r="J71" s="18"/>
       <c r="K71" s="21">
         <v>0.11192322739267201</v>
       </c>
@@ -6141,15 +5724,9 @@
       <c r="G72" s="18">
         <v>1</v>
       </c>
-      <c r="H72" s="17">
-        <v>26</v>
-      </c>
-      <c r="I72" s="20">
-        <v>20.524437716262977</v>
-      </c>
-      <c r="J72" s="18">
-        <v>13</v>
-      </c>
+      <c r="H72" s="17"/>
+      <c r="I72" s="20"/>
+      <c r="J72" s="18"/>
       <c r="K72" s="21">
         <v>4.9979222159862599E-2</v>
       </c>
@@ -6211,15 +5788,9 @@
       <c r="G73" s="18">
         <v>1</v>
       </c>
-      <c r="H73" s="17">
-        <v>20</v>
-      </c>
-      <c r="I73" s="20">
-        <v>25.4375</v>
-      </c>
-      <c r="J73" s="18">
-        <v>16</v>
-      </c>
+      <c r="H73" s="17"/>
+      <c r="I73" s="20"/>
+      <c r="J73" s="18"/>
       <c r="K73" s="21">
         <v>7.0010836564953299E-2</v>
       </c>
@@ -6281,15 +5852,9 @@
       <c r="G74" s="18">
         <v>1</v>
       </c>
-      <c r="H74" s="17">
-        <v>20</v>
-      </c>
-      <c r="I74" s="20">
-        <v>21.824324324324323</v>
-      </c>
-      <c r="J74" s="18">
-        <v>15</v>
-      </c>
+      <c r="H74" s="17"/>
+      <c r="I74" s="20"/>
+      <c r="J74" s="18"/>
       <c r="K74" s="21">
         <v>2.3542686616370899E-2</v>
       </c>
@@ -6351,15 +5916,9 @@
       <c r="G75" s="18">
         <v>1</v>
       </c>
-      <c r="H75" s="17">
-        <v>20</v>
-      </c>
-      <c r="I75" s="22">
-        <v>27.365916955017301</v>
-      </c>
-      <c r="J75" s="18">
-        <v>16</v>
-      </c>
+      <c r="H75" s="17"/>
+      <c r="I75" s="22"/>
+      <c r="J75" s="18"/>
       <c r="K75" s="21">
         <v>3.39986988639348E-2</v>
       </c>
@@ -6421,15 +5980,9 @@
       <c r="G76" s="18">
         <v>1</v>
       </c>
-      <c r="H76" s="17">
-        <v>20</v>
-      </c>
-      <c r="I76" s="20">
-        <v>25.1</v>
-      </c>
-      <c r="J76" s="18">
-        <v>13</v>
-      </c>
+      <c r="H76" s="17"/>
+      <c r="I76" s="20"/>
+      <c r="J76" s="18"/>
       <c r="K76" s="21">
         <v>6.4463827809420698E-2</v>
       </c>
@@ -6491,15 +6044,9 @@
       <c r="G77" s="18">
         <v>1</v>
       </c>
-      <c r="H77" s="17">
-        <v>23</v>
-      </c>
-      <c r="I77" s="20">
-        <v>23.48170388440608</v>
-      </c>
-      <c r="J77" s="18">
-        <v>15</v>
-      </c>
+      <c r="H77" s="17"/>
+      <c r="I77" s="20"/>
+      <c r="J77" s="18"/>
       <c r="K77" s="21">
         <v>3.8307501087284701E-2</v>
       </c>
@@ -6561,15 +6108,9 @@
       <c r="G78" s="18">
         <v>0</v>
       </c>
-      <c r="H78" s="17">
-        <v>28</v>
-      </c>
-      <c r="I78" s="20">
-        <v>25.74462890625</v>
-      </c>
-      <c r="J78" s="18">
-        <v>16</v>
-      </c>
+      <c r="H78" s="17"/>
+      <c r="I78" s="20"/>
+      <c r="J78" s="18"/>
       <c r="K78" s="21">
         <v>7.8162234150491894E-2</v>
       </c>
@@ -6631,15 +6172,9 @@
       <c r="G79" s="18">
         <v>0</v>
       </c>
-      <c r="H79" s="17">
-        <v>18</v>
-      </c>
-      <c r="I79" s="20">
-        <v>20.980257116620752</v>
-      </c>
-      <c r="J79" s="18">
-        <v>13</v>
-      </c>
+      <c r="H79" s="17"/>
+      <c r="I79" s="20"/>
+      <c r="J79" s="18"/>
       <c r="K79" s="21">
         <v>2.5889994600325001E-2</v>
       </c>
@@ -6701,15 +6236,9 @@
       <c r="G80" s="18">
         <v>0</v>
       </c>
-      <c r="H80" s="17">
-        <v>20</v>
-      </c>
-      <c r="I80" s="20">
-        <v>22.462721893491121</v>
-      </c>
-      <c r="J80" s="18">
-        <v>15</v>
-      </c>
+      <c r="H80" s="17"/>
+      <c r="I80" s="20"/>
+      <c r="J80" s="18"/>
       <c r="K80" s="21">
         <v>5.3182637233523802E-2</v>
       </c>
@@ -6771,15 +6300,9 @@
       <c r="G81" s="18">
         <v>0</v>
       </c>
-      <c r="H81" s="17">
-        <v>25</v>
-      </c>
-      <c r="I81" s="20">
-        <v>19.483497102544721</v>
-      </c>
-      <c r="J81" s="18">
-        <v>17</v>
-      </c>
+      <c r="H81" s="17"/>
+      <c r="I81" s="20"/>
+      <c r="J81" s="18"/>
       <c r="K81" s="21">
         <v>3.8856355111128997E-2</v>
       </c>
@@ -6841,15 +6364,9 @@
       <c r="G82" s="18">
         <v>1</v>
       </c>
-      <c r="H82" s="17">
-        <v>18</v>
-      </c>
-      <c r="I82" s="20">
-        <v>20.980257116620752</v>
-      </c>
-      <c r="J82" s="18">
-        <v>13</v>
-      </c>
+      <c r="H82" s="17"/>
+      <c r="I82" s="20"/>
+      <c r="J82" s="18"/>
       <c r="K82" s="21">
         <v>5.8320973278282097E-2</v>
       </c>
@@ -6911,15 +6428,9 @@
       <c r="G83" s="18">
         <v>1</v>
       </c>
-      <c r="H83" s="17">
-        <v>19</v>
-      </c>
-      <c r="I83" s="20">
-        <v>25.84558823529412</v>
-      </c>
-      <c r="J83" s="18">
-        <v>14</v>
-      </c>
+      <c r="H83" s="17"/>
+      <c r="I83" s="20"/>
+      <c r="J83" s="18"/>
       <c r="K83" s="21">
         <v>4.0052881087290902E-2</v>
       </c>
@@ -6981,15 +6492,9 @@
       <c r="G84" s="18">
         <v>1</v>
       </c>
-      <c r="H84" s="17">
-        <v>19</v>
-      </c>
-      <c r="I84" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="J84" s="18">
-        <v>13</v>
-      </c>
+      <c r="H84" s="17"/>
+      <c r="I84" s="18"/>
+      <c r="J84" s="18"/>
       <c r="K84" s="21">
         <v>2.5732549390204699E-2</v>
       </c>
@@ -7051,15 +6556,9 @@
       <c r="G85" s="18">
         <v>1</v>
       </c>
-      <c r="H85" s="17">
-        <v>20</v>
-      </c>
-      <c r="I85" s="20">
-        <v>26.44386574074074</v>
-      </c>
-      <c r="J85" s="18">
-        <v>15</v>
-      </c>
+      <c r="H85" s="17"/>
+      <c r="I85" s="20"/>
+      <c r="J85" s="18"/>
       <c r="K85" s="21">
         <v>0.15650684575711199</v>
       </c>
@@ -7121,15 +6620,9 @@
       <c r="G86" s="18">
         <v>1</v>
       </c>
-      <c r="H86" s="17">
-        <v>30</v>
-      </c>
-      <c r="I86" s="20">
-        <v>24.781358131487888</v>
-      </c>
-      <c r="J86" s="18">
-        <v>19</v>
-      </c>
+      <c r="H86" s="17"/>
+      <c r="I86" s="20"/>
+      <c r="J86" s="18"/>
       <c r="K86" s="21">
         <v>3.9958334015082198E-2</v>
       </c>
@@ -7191,15 +6684,9 @@
       <c r="G87" s="18">
         <v>1</v>
       </c>
-      <c r="H87" s="17">
-        <v>29</v>
-      </c>
-      <c r="I87" s="20">
-        <v>22.375578703703706</v>
-      </c>
-      <c r="J87" s="18">
-        <v>19</v>
-      </c>
+      <c r="H87" s="17"/>
+      <c r="I87" s="20"/>
+      <c r="J87" s="18"/>
       <c r="K87" s="21">
         <v>2.4484068449769102E-2</v>
       </c>
@@ -7261,15 +6748,9 @@
       <c r="G88" s="18">
         <v>0</v>
       </c>
-      <c r="H88" s="17">
-        <v>19</v>
-      </c>
-      <c r="I88" s="20">
-        <v>19.483497102544721</v>
-      </c>
-      <c r="J88" s="18">
-        <v>14</v>
-      </c>
+      <c r="H88" s="17"/>
+      <c r="I88" s="20"/>
+      <c r="J88" s="18"/>
       <c r="K88" s="21">
         <v>6.9112524520301796E-2</v>
       </c>
@@ -7331,15 +6812,9 @@
       <c r="G89" s="18">
         <v>0</v>
       </c>
-      <c r="H89" s="17">
-        <v>33</v>
-      </c>
-      <c r="I89" s="20">
-        <v>18.792604143461794</v>
-      </c>
-      <c r="J89" s="18">
-        <v>16</v>
-      </c>
+      <c r="H89" s="17"/>
+      <c r="I89" s="20"/>
+      <c r="J89" s="18"/>
       <c r="K89" s="21">
         <v>8.8740778505300794E-2</v>
       </c>
@@ -7401,15 +6876,9 @@
       <c r="G90" s="18">
         <v>0</v>
       </c>
-      <c r="H90" s="17">
-        <v>26</v>
-      </c>
-      <c r="I90" s="20">
-        <v>25.83983069725997</v>
-      </c>
-      <c r="J90" s="18">
-        <v>16</v>
-      </c>
+      <c r="H90" s="17"/>
+      <c r="I90" s="20"/>
+      <c r="J90" s="18"/>
       <c r="K90" s="21">
         <v>4.9321799678997899E-2</v>
       </c>
@@ -7471,15 +6940,9 @@
       <c r="G91" s="18">
         <v>1</v>
       </c>
-      <c r="H91" s="17">
-        <v>22</v>
-      </c>
-      <c r="I91" s="20">
-        <v>20.524437716262977</v>
-      </c>
-      <c r="J91" s="18">
-        <v>17</v>
-      </c>
+      <c r="H91" s="17"/>
+      <c r="I91" s="20"/>
+      <c r="J91" s="18"/>
       <c r="K91" s="21">
         <v>5.5617795664457403E-2</v>
       </c>
@@ -7541,15 +7004,9 @@
       <c r="G92" s="18">
         <v>0</v>
       </c>
-      <c r="H92" s="17">
-        <v>19</v>
-      </c>
-      <c r="I92" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="J92" s="18">
-        <v>13</v>
-      </c>
+      <c r="H92" s="17"/>
+      <c r="I92" s="18"/>
+      <c r="J92" s="18"/>
       <c r="K92" s="21">
         <v>4.4213101192982801E-2</v>
       </c>
@@ -7611,15 +7068,9 @@
       <c r="G93" s="18">
         <v>0</v>
       </c>
-      <c r="H93" s="17">
-        <v>23</v>
-      </c>
-      <c r="I93" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="J93" s="18">
-        <v>17</v>
-      </c>
+      <c r="H93" s="17"/>
+      <c r="I93" s="18"/>
+      <c r="J93" s="18"/>
       <c r="K93" s="21">
         <v>0.13144785039652401</v>
       </c>
@@ -7681,15 +7132,9 @@
       <c r="G94" s="18">
         <v>1</v>
       </c>
-      <c r="H94" s="17">
-        <v>21</v>
-      </c>
-      <c r="I94" s="20">
-        <v>23.611842105263158</v>
-      </c>
-      <c r="J94" s="18">
-        <v>16</v>
-      </c>
+      <c r="H94" s="17"/>
+      <c r="I94" s="20"/>
+      <c r="J94" s="18"/>
       <c r="K94" s="21">
         <v>3.0654160415504599E-2</v>
       </c>
@@ -7751,15 +7196,9 @@
       <c r="G95" s="18">
         <v>1</v>
       </c>
-      <c r="H95" s="17">
-        <v>18</v>
-      </c>
-      <c r="I95" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="J95" s="18">
-        <v>13</v>
-      </c>
+      <c r="H95" s="17"/>
+      <c r="I95" s="18"/>
+      <c r="J95" s="18"/>
       <c r="K95" s="21">
         <v>2.9033474520922201E-2</v>
       </c>
@@ -7821,15 +7260,9 @@
       <c r="G96" s="18">
         <v>1</v>
       </c>
-      <c r="H96" s="17">
-        <v>38</v>
-      </c>
-      <c r="I96" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="J96" s="18">
-        <v>16</v>
-      </c>
+      <c r="H96" s="17"/>
+      <c r="I96" s="18"/>
+      <c r="J96" s="18"/>
       <c r="K96" s="21">
         <v>0.21440436653254899</v>
       </c>
@@ -7891,15 +7324,9 @@
       <c r="G97" s="18">
         <v>0</v>
       </c>
-      <c r="H97" s="17">
-        <v>22</v>
-      </c>
-      <c r="I97" s="20">
-        <v>24.0283203125</v>
-      </c>
-      <c r="J97" s="18">
-        <v>17</v>
-      </c>
+      <c r="H97" s="17"/>
+      <c r="I97" s="20"/>
+      <c r="J97" s="18"/>
       <c r="K97" s="21">
         <v>4.0307995101945E-2</v>
       </c>
@@ -7961,15 +7388,9 @@
       <c r="G98" s="18">
         <v>1</v>
       </c>
-      <c r="H98" s="17">
-        <v>34</v>
-      </c>
-      <c r="I98" s="20">
-        <v>21.907894736842106</v>
-      </c>
-      <c r="J98" s="18">
-        <v>17</v>
-      </c>
+      <c r="H98" s="17"/>
+      <c r="I98" s="20"/>
+      <c r="J98" s="18"/>
       <c r="K98" s="21">
         <v>4.8193519906085502E-2</v>
       </c>
@@ -8031,15 +7452,9 @@
       <c r="G99" s="18">
         <v>1</v>
       </c>
-      <c r="H99" s="18">
-        <v>41</v>
-      </c>
-      <c r="I99" s="20">
-        <v>27.194009125173579</v>
-      </c>
-      <c r="J99" s="18">
-        <v>15</v>
-      </c>
+      <c r="H99" s="18"/>
+      <c r="I99" s="20"/>
+      <c r="J99" s="18"/>
       <c r="K99" s="21">
         <v>0.121546712563758</v>
       </c>
@@ -8101,15 +7516,9 @@
       <c r="G100" s="18">
         <v>0</v>
       </c>
-      <c r="H100" s="18">
-        <v>40</v>
-      </c>
-      <c r="I100" s="20">
-        <v>23.75</v>
-      </c>
-      <c r="J100" s="18">
-        <v>15</v>
-      </c>
+      <c r="H100" s="18"/>
+      <c r="I100" s="20"/>
+      <c r="J100" s="18"/>
       <c r="K100" s="21">
         <v>5.6719969244588803E-2</v>
       </c>
@@ -8171,15 +7580,9 @@
       <c r="G101" s="18">
         <v>1</v>
       </c>
-      <c r="H101" s="18">
-        <v>44</v>
-      </c>
-      <c r="I101" s="20">
-        <v>24.743595455558033</v>
-      </c>
-      <c r="J101" s="18">
-        <v>16</v>
-      </c>
+      <c r="H101" s="18"/>
+      <c r="I101" s="20"/>
+      <c r="J101" s="18"/>
       <c r="K101" s="21">
         <v>4.1522058747002301E-2</v>
       </c>

</xml_diff>